<commit_message>
Added new aerofoils to JavaFoilData.m
</commit_message>
<xml_diff>
--- a/data/Clark Y.xlsx
+++ b/data/Clark Y.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Downloads\ADOT_OO_14_12_2023_1.15_PM\ADOT 2023\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2ACFA108-22D6-4FCA-A3B8-09B5073CEE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53725EE-288F-443A-ABC4-306106267BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1032" yWindow="228" windowWidth="21624" windowHeight="11220" activeTab="3" xr2:uid="{DAD8838B-BAF3-4F72-A12F-8880791810A1}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="19680" windowHeight="16395" xr2:uid="{DAD8838B-BAF3-4F72-A12F-8880791810A1}"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="19">
   <si>
     <t>Name = Clark Y</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>30 degree flap deflection</t>
+  </si>
+  <si>
+    <t>Max_Thickness</t>
   </si>
 </sst>
 </file>
@@ -444,30 +447,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9216384-01B3-432B-A983-B06C38BF3E4E}">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -501,8 +504,11 @@
       <c r="K4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -536,8 +542,11 @@
       <c r="K5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>0.11700000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-30</v>
       </c>
@@ -572,7 +581,7 @@
         <v>0.124</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-29</v>
       </c>
@@ -607,7 +616,7 @@
         <v>0.13200000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-28</v>
       </c>
@@ -642,7 +651,7 @@
         <v>0.13900000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-27</v>
       </c>
@@ -677,7 +686,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-26</v>
       </c>
@@ -712,7 +721,7 @@
         <v>0.151</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-25</v>
       </c>
@@ -747,7 +756,7 @@
         <v>0.156</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-24</v>
       </c>
@@ -782,7 +791,7 @@
         <v>0.161</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-23</v>
       </c>
@@ -817,7 +826,7 @@
         <v>0.16600000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-22</v>
       </c>
@@ -852,7 +861,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-21</v>
       </c>
@@ -887,7 +896,7 @@
         <v>0.17399999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-20</v>
       </c>
@@ -922,7 +931,7 @@
         <v>0.17699999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-19</v>
       </c>
@@ -957,7 +966,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-18</v>
       </c>
@@ -992,7 +1001,7 @@
         <v>0.182</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-17</v>
       </c>
@@ -1027,7 +1036,7 @@
         <v>0.18099999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-16</v>
       </c>
@@ -1062,7 +1071,7 @@
         <v>0.18099999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-15</v>
       </c>
@@ -1097,7 +1106,7 @@
         <v>0.17899999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-14</v>
       </c>
@@ -1132,7 +1141,7 @@
         <v>0.17699999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-13</v>
       </c>
@@ -1167,7 +1176,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-12</v>
       </c>
@@ -1202,7 +1211,7 @@
         <v>0.14699999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-11</v>
       </c>
@@ -1237,7 +1246,7 @@
         <v>0.13300000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-10</v>
       </c>
@@ -1272,7 +1281,7 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-9</v>
       </c>
@@ -1307,7 +1316,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-8</v>
       </c>
@@ -1342,7 +1351,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-7</v>
       </c>
@@ -1377,7 +1386,7 @@
         <v>-6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-6</v>
       </c>
@@ -1412,7 +1421,7 @@
         <v>-0.14599999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-5</v>
       </c>
@@ -1447,7 +1456,7 @@
         <v>-0.625</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-4</v>
       </c>
@@ -1482,7 +1491,7 @@
         <v>4.3550000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-3</v>
       </c>
@@ -1517,7 +1526,7 @@
         <v>0.86699999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-2</v>
       </c>
@@ -1552,7 +1561,7 @@
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-1</v>
       </c>
@@ -1587,7 +1596,7 @@
         <v>0.48199999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -1622,7 +1631,7 @@
         <v>0.42799999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1657,7 +1666,7 @@
         <v>0.39500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1692,7 +1701,7 @@
         <v>0.373</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -1727,7 +1736,7 @@
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1762,7 +1771,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>
@@ -1797,7 +1806,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
@@ -1832,7 +1841,7 @@
         <v>0.32800000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7</v>
       </c>
@@ -1867,7 +1876,7 @@
         <v>0.32200000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>8</v>
       </c>
@@ -1902,7 +1911,7 @@
         <v>0.318</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9</v>
       </c>
@@ -1937,7 +1946,7 @@
         <v>0.315</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>10</v>
       </c>
@@ -1972,7 +1981,7 @@
         <v>0.313</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>11</v>
       </c>
@@ -2007,7 +2016,7 @@
         <v>0.312</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>12</v>
       </c>
@@ -2042,7 +2051,7 @@
         <v>0.312</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>13</v>
       </c>
@@ -2077,7 +2086,7 @@
         <v>0.313</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>14</v>
       </c>
@@ -2112,7 +2121,7 @@
         <v>0.315</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15</v>
       </c>
@@ -2147,7 +2156,7 @@
         <v>0.318</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>16</v>
       </c>
@@ -2182,7 +2191,7 @@
         <v>0.32100000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>17</v>
       </c>
@@ -2217,7 +2226,7 @@
         <v>0.32600000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>18</v>
       </c>
@@ -2252,7 +2261,7 @@
         <v>0.33100000000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>19</v>
       </c>
@@ -2287,7 +2296,7 @@
         <v>0.33600000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20</v>
       </c>
@@ -2322,7 +2331,7 @@
         <v>0.34300000000000003</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>21</v>
       </c>
@@ -2357,7 +2366,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>22</v>
       </c>
@@ -2392,7 +2401,7 @@
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>23</v>
       </c>
@@ -2427,7 +2436,7 @@
         <v>0.36499999999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>24</v>
       </c>
@@ -2462,7 +2471,7 @@
         <v>0.374</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>25</v>
       </c>
@@ -2497,7 +2506,7 @@
         <v>0.38500000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>26</v>
       </c>
@@ -2532,7 +2541,7 @@
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>27</v>
       </c>
@@ -2567,7 +2576,7 @@
         <v>0.40699999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>28</v>
       </c>
@@ -2602,7 +2611,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>29</v>
       </c>
@@ -2637,7 +2646,7 @@
         <v>0.433</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>30</v>
       </c>
@@ -2685,9 +2694,9 @@
       <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2707,7 +2716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2718,7 +2727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2729,7 +2738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2830,7 +2839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2931,7 +2940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-30</v>
       </c>
@@ -3032,7 +3041,7 @@
         <v>-0.20200000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-29</v>
       </c>
@@ -3133,7 +3142,7 @@
         <v>-0.19500000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-28</v>
       </c>
@@ -3234,7 +3243,7 @@
         <v>-0.187</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-27</v>
       </c>
@@ -3335,7 +3344,7 @@
         <v>-0.182</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-26</v>
       </c>
@@ -3436,7 +3445,7 @@
         <v>-0.18</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-25</v>
       </c>
@@ -3537,7 +3546,7 @@
         <v>-0.183</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-24</v>
       </c>
@@ -3638,7 +3647,7 @@
         <v>-0.193</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-23</v>
       </c>
@@ -3739,7 +3748,7 @@
         <v>-0.218</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-22</v>
       </c>
@@ -3840,7 +3849,7 @@
         <v>-0.25800000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-21</v>
       </c>
@@ -3941,7 +3950,7 @@
         <v>-0.32300000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-20</v>
       </c>
@@ -4042,7 +4051,7 @@
         <v>-0.44</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-19</v>
       </c>
@@ -4143,7 +4152,7 @@
         <v>-0.64200000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-18</v>
       </c>
@@ -4244,7 +4253,7 @@
         <v>-1.177</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-17</v>
       </c>
@@ -4345,7 +4354,7 @@
         <v>-2.87</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-16</v>
       </c>
@@ -4446,7 +4455,7 @@
         <v>67.277000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-15</v>
       </c>
@@ -4547,7 +4556,7 @@
         <v>3.0129999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-14</v>
       </c>
@@ -4648,7 +4657,7 @@
         <v>1.639</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-13</v>
       </c>
@@ -4749,7 +4758,7 @@
         <v>1.175</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-12</v>
       </c>
@@ -4850,7 +4859,7 @@
         <v>0.94299999999999995</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-11</v>
       </c>
@@ -4951,7 +4960,7 @@
         <v>0.79600000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-10</v>
       </c>
@@ -5052,7 +5061,7 @@
         <v>0.70899999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-9</v>
       </c>
@@ -5153,7 +5162,7 @@
         <v>0.64600000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-8</v>
       </c>
@@ -5254,7 +5263,7 @@
         <v>0.59899999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-7</v>
       </c>
@@ -5355,7 +5364,7 @@
         <v>0.56200000000000006</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-6</v>
       </c>
@@ -5456,7 +5465,7 @@
         <v>0.53200000000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-5</v>
       </c>
@@ -5557,7 +5566,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-4</v>
       </c>
@@ -5658,7 +5667,7 @@
         <v>0.48699999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-3</v>
       </c>
@@ -5759,7 +5768,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-2</v>
       </c>
@@ -5860,7 +5869,7 @@
         <v>0.45500000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-1</v>
       </c>
@@ -5961,7 +5970,7 @@
         <v>0.442</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -6062,7 +6071,7 @@
         <v>0.42699999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -6163,7 +6172,7 @@
         <v>0.41699999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -6264,7 +6273,7 @@
         <v>0.41499999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -6365,7 +6374,7 @@
         <v>0.41099999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -6466,7 +6475,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>
@@ -6567,7 +6576,7 @@
         <v>0.40699999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
@@ -6668,7 +6677,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7</v>
       </c>
@@ -6769,7 +6778,7 @@
         <v>0.41199999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>8</v>
       </c>
@@ -6870,7 +6879,7 @@
         <v>0.41699999999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9</v>
       </c>
@@ -6971,7 +6980,7 @@
         <v>0.42399999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>10</v>
       </c>
@@ -7072,7 +7081,7 @@
         <v>0.434</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>11</v>
       </c>
@@ -7173,7 +7182,7 @@
         <v>0.44600000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>12</v>
       </c>
@@ -7274,7 +7283,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>13</v>
       </c>
@@ -7375,7 +7384,7 @@
         <v>0.47599999999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>14</v>
       </c>
@@ -7476,7 +7485,7 @@
         <v>0.495</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15</v>
       </c>
@@ -7577,7 +7586,7 @@
         <v>0.51600000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>16</v>
       </c>
@@ -7678,7 +7687,7 @@
         <v>0.53600000000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>17</v>
       </c>
@@ -7779,7 +7788,7 @@
         <v>0.55700000000000005</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>18</v>
       </c>
@@ -7880,7 +7889,7 @@
         <v>0.57799999999999996</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>19</v>
       </c>
@@ -7981,7 +7990,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20</v>
       </c>
@@ -8082,7 +8091,7 @@
         <v>0.621</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>21</v>
       </c>
@@ -8183,7 +8192,7 @@
         <v>0.64600000000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>22</v>
       </c>
@@ -8284,7 +8293,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>23</v>
       </c>
@@ -8385,7 +8394,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>24</v>
       </c>
@@ -8486,7 +8495,7 @@
         <v>0.73399999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>25</v>
       </c>
@@ -8587,7 +8596,7 @@
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>26</v>
       </c>
@@ -8688,7 +8697,7 @@
         <v>0.79500000000000004</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>27</v>
       </c>
@@ -8789,7 +8798,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>28</v>
       </c>
@@ -8890,7 +8899,7 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>29</v>
       </c>
@@ -8991,7 +9000,7 @@
         <v>0.88700000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>30</v>
       </c>
@@ -9105,9 +9114,9 @@
       <selection sqref="A1:AA1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9127,7 +9136,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -9138,7 +9147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9149,7 +9158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -9250,7 +9259,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -9351,7 +9360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-30</v>
       </c>
@@ -9452,7 +9461,7 @@
         <v>-0.31900000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-29</v>
       </c>
@@ -9553,7 +9562,7 @@
         <v>-0.32900000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-28</v>
       </c>
@@ -9654,7 +9663,7 @@
         <v>-0.35399999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-27</v>
       </c>
@@ -9755,7 +9764,7 @@
         <v>-0.39200000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-26</v>
       </c>
@@ -9856,7 +9865,7 @@
         <v>-0.45500000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-25</v>
       </c>
@@ -9957,7 +9966,7 @@
         <v>-0.57499999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-24</v>
       </c>
@@ -10058,7 +10067,7 @@
         <v>-0.77100000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-23</v>
       </c>
@@ -10159,7 +10168,7 @@
         <v>-1.194</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-22</v>
       </c>
@@ -10260,7 +10269,7 @@
         <v>-2.4340000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-21</v>
       </c>
@@ -10361,7 +10370,7 @@
         <v>-35.503999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-20</v>
       </c>
@@ -10462,7 +10471,7 @@
         <v>3.649</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-19</v>
       </c>
@@ -10563,7 +10572,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-18</v>
       </c>
@@ -10664,7 +10673,7 @@
         <v>1.3520000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-17</v>
       </c>
@@ -10765,7 +10774,7 @@
         <v>1.0629999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-16</v>
       </c>
@@ -10866,7 +10875,7 @@
         <v>0.89400000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-15</v>
       </c>
@@ -10967,7 +10976,7 @@
         <v>0.76900000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-14</v>
       </c>
@@ -11068,7 +11077,7 @@
         <v>0.69399999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-13</v>
       </c>
@@ -11169,7 +11178,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-12</v>
       </c>
@@ -11270,7 +11279,7 @@
         <v>0.59399999999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-11</v>
       </c>
@@ -11371,7 +11380,7 @@
         <v>0.56399999999999995</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-10</v>
       </c>
@@ -11472,7 +11481,7 @@
         <v>0.53700000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-9</v>
       </c>
@@ -11573,7 +11582,7 @@
         <v>0.51400000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-8</v>
       </c>
@@ -11674,7 +11683,7 @@
         <v>0.495</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-7</v>
       </c>
@@ -11775,7 +11784,7 @@
         <v>0.47799999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-6</v>
       </c>
@@ -11876,7 +11885,7 @@
         <v>0.46400000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-5</v>
       </c>
@@ -11977,7 +11986,7 @@
         <v>0.45100000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-4</v>
       </c>
@@ -12078,7 +12087,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-3</v>
       </c>
@@ -12179,7 +12188,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-2</v>
       </c>
@@ -12280,7 +12289,7 @@
         <v>0.42099999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-1</v>
       </c>
@@ -12381,7 +12390,7 @@
         <v>0.41199999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -12482,7 +12491,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -12583,7 +12592,7 @@
         <v>0.40699999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -12684,7 +12693,7 @@
         <v>0.40699999999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -12785,7 +12794,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -12886,7 +12895,7 @@
         <v>0.41099999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>
@@ -12987,7 +12996,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
@@ -13088,7 +13097,7 @@
         <v>0.42299999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7</v>
       </c>
@@ -13189,7 +13198,7 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>8</v>
       </c>
@@ -13290,7 +13299,7 @@
         <v>0.44400000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9</v>
       </c>
@@ -13391,7 +13400,7 @@
         <v>0.45700000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>10</v>
       </c>
@@ -13492,7 +13501,7 @@
         <v>0.47299999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>11</v>
       </c>
@@ -13593,7 +13602,7 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>12</v>
       </c>
@@ -13694,7 +13703,7 @@
         <v>0.51200000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>13</v>
       </c>
@@ -13795,7 +13804,7 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>14</v>
       </c>
@@ -13896,7 +13905,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15</v>
       </c>
@@ -13997,7 +14006,7 @@
         <v>0.58699999999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>16</v>
       </c>
@@ -14098,7 +14107,7 @@
         <v>0.61699999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>17</v>
       </c>
@@ -14199,7 +14208,7 @@
         <v>0.63500000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>18</v>
       </c>
@@ -14300,7 +14309,7 @@
         <v>0.65800000000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>19</v>
       </c>
@@ -14401,7 +14410,7 @@
         <v>0.68100000000000005</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20</v>
       </c>
@@ -14502,7 +14511,7 @@
         <v>0.70799999999999996</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>21</v>
       </c>
@@ -14603,7 +14612,7 @@
         <v>0.73899999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>22</v>
       </c>
@@ -14704,7 +14713,7 @@
         <v>0.77200000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>23</v>
       </c>
@@ -14805,7 +14814,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>24</v>
       </c>
@@ -14906,7 +14915,7 @@
         <v>0.83599999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>25</v>
       </c>
@@ -15007,7 +15016,7 @@
         <v>0.86799999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>26</v>
       </c>
@@ -15108,7 +15117,7 @@
         <v>0.89800000000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>27</v>
       </c>
@@ -15209,7 +15218,7 @@
         <v>0.92900000000000005</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>28</v>
       </c>
@@ -15310,7 +15319,7 @@
         <v>0.96099999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>29</v>
       </c>
@@ -15411,7 +15420,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>30</v>
       </c>
@@ -15521,13 +15530,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C841910-F9AA-4BC6-B4E3-286001C8B2A8}">
   <dimension ref="A1:AI66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15547,7 +15556,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -15558,7 +15567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -15569,7 +15578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -15670,7 +15679,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -15771,7 +15780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-30</v>
       </c>
@@ -15872,7 +15881,7 @@
         <v>-0.47</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-29</v>
       </c>
@@ -15973,7 +15982,7 @@
         <v>-0.56000000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-28</v>
       </c>
@@ -16074,7 +16083,7 @@
         <v>-0.70599999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-27</v>
       </c>
@@ -16175,7 +16184,7 @@
         <v>-1.0029999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-26</v>
       </c>
@@ -16276,7 +16285,7 @@
         <v>-1.752</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-25</v>
       </c>
@@ -16377,7 +16386,7 @@
         <v>-5.5570000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-24</v>
       </c>
@@ -16478,7 +16487,7 @@
         <v>5.6369999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-23</v>
       </c>
@@ -16579,7 +16588,7 @@
         <v>2.0830000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-22</v>
       </c>
@@ -16680,7 +16689,7 @@
         <v>1.4219999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-21</v>
       </c>
@@ -16781,7 +16790,7 @@
         <v>1.115</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-20</v>
       </c>
@@ -16882,7 +16891,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-19</v>
       </c>
@@ -16983,7 +16992,7 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-18</v>
       </c>
@@ -17084,7 +17093,7 @@
         <v>0.71799999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-17</v>
       </c>
@@ -17185,7 +17194,7 @@
         <v>0.64700000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-16</v>
       </c>
@@ -17286,7 +17295,7 @@
         <v>0.60399999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-15</v>
       </c>
@@ -17387,7 +17396,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-14</v>
       </c>
@@ -17488,7 +17497,7 @@
         <v>0.54200000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-13</v>
       </c>
@@ -17589,7 +17598,7 @@
         <v>0.51800000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-12</v>
       </c>
@@ -17690,7 +17699,7 @@
         <v>0.498</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-11</v>
       </c>
@@ -17791,7 +17800,7 @@
         <v>0.47399999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-10</v>
       </c>
@@ -17892,7 +17901,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-9</v>
       </c>
@@ -17993,7 +18002,7 @@
         <v>0.44700000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-8</v>
       </c>
@@ -18094,7 +18103,7 @@
         <v>0.436</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-7</v>
       </c>
@@ -18195,7 +18204,7 @@
         <v>0.42599999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-6</v>
       </c>
@@ -18296,7 +18305,7 @@
         <v>0.41699999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-5</v>
       </c>
@@ -18397,7 +18406,7 @@
         <v>0.40899999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-4</v>
       </c>
@@ -18498,7 +18507,7 @@
         <v>0.40100000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-3</v>
       </c>
@@ -18599,7 +18608,7 @@
         <v>0.39500000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-2</v>
       </c>
@@ -18700,7 +18709,7 @@
         <v>0.39700000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-1</v>
       </c>
@@ -18801,7 +18810,7 @@
         <v>0.39500000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0</v>
       </c>
@@ -18902,7 +18911,7 @@
         <v>0.39100000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -19003,7 +19012,7 @@
         <v>0.39200000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -19104,7 +19113,7 @@
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -19205,7 +19214,7 @@
         <v>0.40100000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -19306,7 +19315,7 @@
         <v>0.40699999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>
@@ -19407,7 +19416,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
@@ -19508,7 +19517,7 @@
         <v>0.42699999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7</v>
       </c>
@@ -19609,7 +19618,7 @@
         <v>0.439</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>8</v>
       </c>
@@ -19710,7 +19719,7 @@
         <v>0.45400000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9</v>
       </c>
@@ -19811,7 +19820,7 @@
         <v>0.47099999999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>10</v>
       </c>
@@ -19912,7 +19921,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>11</v>
       </c>
@@ -20013,7 +20022,7 @@
         <v>0.51100000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>12</v>
       </c>
@@ -20114,7 +20123,7 @@
         <v>0.53400000000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>13</v>
       </c>
@@ -20215,7 +20224,7 @@
         <v>0.55900000000000005</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>14</v>
       </c>
@@ -20316,7 +20325,7 @@
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15</v>
       </c>
@@ -20417,7 +20426,7 @@
         <v>0.61399999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>16</v>
       </c>
@@ -20518,7 +20527,7 @@
         <v>0.64500000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>17</v>
       </c>
@@ -20619,7 +20628,7 @@
         <v>0.66200000000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>18</v>
       </c>
@@ -20720,7 +20729,7 @@
         <v>0.67900000000000005</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>19</v>
       </c>
@@ -20821,7 +20830,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20</v>
       </c>
@@ -20922,7 +20931,7 @@
         <v>0.73299999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>21</v>
       </c>
@@ -21023,7 +21032,7 @@
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>22</v>
       </c>
@@ -21124,7 +21133,7 @@
         <v>0.79200000000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>23</v>
       </c>
@@ -21225,7 +21234,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>24</v>
       </c>
@@ -21326,7 +21335,7 @@
         <v>0.84899999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>25</v>
       </c>
@@ -21427,7 +21436,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>26</v>
       </c>
@@ -21528,7 +21537,7 @@
         <v>0.90500000000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>27</v>
       </c>
@@ -21629,7 +21638,7 @@
         <v>0.93300000000000005</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>28</v>
       </c>
@@ -21730,7 +21739,7 @@
         <v>0.96199999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>29</v>
       </c>
@@ -21831,7 +21840,7 @@
         <v>0.99299999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>30</v>
       </c>

</xml_diff>